<commit_message>
Intégrer propositions Saint-Nazaire, Colmar, Valence
- Saint-Nazaire : 33 propositions Violaine Lucas (sn26.fr, programmeComplet)
- Colmar : 10 propositions Yves Hémedinger (yhcolmar2026.fr)
- Valence : 21 propositions Paul Christophle (reunirvalence.fr, programmeComplet)
- Correction attribution URL reunirvalence.fr (Christophle, pas Boyadjian)
- Régénération Excel programmes

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/docs/programmes-candidats-2026.xlsx
+++ b/docs/programmes-candidats-2026.xlsx
@@ -5102,13 +5102,13 @@
           <t>https://yhcolmar2026.fr/</t>
         </is>
       </c>
-      <c r="F145" s="21" t="inlineStr">
-        <is>
-          <t>Site identifie</t>
+      <c r="F145" s="15" t="inlineStr">
+        <is>
+          <t>Bien couvert</t>
         </is>
       </c>
       <c r="G145" s="16" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H145" s="16" t="inlineStr">
         <is>
@@ -13755,20 +13755,20 @@
       <c r="D445" s="14" t="inlineStr"/>
       <c r="E445" s="17" t="inlineStr">
         <is>
-          <t>https://sn26.fr/</t>
-        </is>
-      </c>
-      <c r="F445" s="21" t="inlineStr">
-        <is>
-          <t>Site identifie</t>
+          <t>https://sn26.fr/programme/</t>
+        </is>
+      </c>
+      <c r="F445" s="20" t="inlineStr">
+        <is>
+          <t>Programme complet</t>
         </is>
       </c>
       <c r="G445" s="16" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="H445" s="16" t="inlineStr">
         <is>
-          <t>Non</t>
+          <t>Oui</t>
         </is>
       </c>
     </row>
@@ -15725,18 +15725,22 @@
       </c>
       <c r="C513" s="14" t="inlineStr"/>
       <c r="D513" s="14" t="inlineStr"/>
-      <c r="E513" s="14" t="inlineStr"/>
-      <c r="F513" s="19" t="inlineStr">
-        <is>
-          <t>En attente</t>
+      <c r="E513" s="17" t="inlineStr">
+        <is>
+          <t>https://reunirvalence.fr/</t>
+        </is>
+      </c>
+      <c r="F513" s="20" t="inlineStr">
+        <is>
+          <t>Programme complet</t>
         </is>
       </c>
       <c r="G513" s="16" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="H513" s="16" t="inlineStr">
         <is>
-          <t>Non</t>
+          <t>Oui</t>
         </is>
       </c>
     </row>
@@ -15753,14 +15757,10 @@
       </c>
       <c r="C514" s="14" t="inlineStr"/>
       <c r="D514" s="14" t="inlineStr"/>
-      <c r="E514" s="17" t="inlineStr">
-        <is>
-          <t>https://reunirvalence.fr/</t>
-        </is>
-      </c>
-      <c r="F514" s="21" t="inlineStr">
-        <is>
-          <t>Site identifie</t>
+      <c r="E514" s="14" t="inlineStr"/>
+      <c r="F514" s="19" t="inlineStr">
+        <is>
+          <t>En attente</t>
         </is>
       </c>
       <c r="G514" s="16" t="n">
@@ -17523,7 +17523,7 @@
         <v>7</v>
       </c>
       <c r="C30" s="16" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D30" s="16" t="n">
         <v>0</v>
@@ -17531,9 +17531,9 @@
       <c r="E30" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="F30" s="19" t="inlineStr">
-        <is>
-          <t>En attente</t>
+      <c r="F30" s="18" t="inlineStr">
+        <is>
+          <t>Partiellement couvert</t>
         </is>
       </c>
     </row>
@@ -18867,17 +18867,17 @@
         <v>4</v>
       </c>
       <c r="C86" s="16" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="D86" s="16" t="n">
         <v>0</v>
       </c>
       <c r="E86" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="F86" s="19" t="inlineStr">
-        <is>
-          <t>En attente</t>
+        <v>1</v>
+      </c>
+      <c r="F86" s="20" t="inlineStr">
+        <is>
+          <t>Programme(s) complet(s)</t>
         </is>
       </c>
     </row>
@@ -19107,17 +19107,17 @@
         <v>6</v>
       </c>
       <c r="C96" s="16" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="D96" s="16" t="n">
         <v>0</v>
       </c>
       <c r="E96" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="F96" s="19" t="inlineStr">
-        <is>
-          <t>En attente</t>
+        <v>1</v>
+      </c>
+      <c r="F96" s="20" t="inlineStr">
+        <is>
+          <t>Programme(s) complet(s)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Intégrer 195 propositions pour 11 candidats dans 8 villes
Villes avec programmes complets :
- Annecy : Armand (25 props, acteursannecy.fr) + Roit-Lévêque (21, retrouvons-annecy.fr)
- Chambéry : Bernard (27 props, brice-bernard.fr)
- Issy-les-Moulineaux : Morel (21 props, issyecoloetsocial.fr)

Villes avec propositions partielles :
- Vitry-sur-Seine : Bell-Lloch (13, pbl2026.fr) + Tmimi (22, vitry2026.fr)
- La Seyne-sur-Mer : Minniti (19, josephminniti2026.fr) + Mansour (14)
- Évry-Courcouronnes : Amrani (10, faridaamrani2026.fr)
- Fréjus : Bonnemain (14, notreparticestfrejus.fr)
- Antony : Precetti (10, antonyavenir.fr)
- Rueil-Malmaison : Indjian (19, patrickindjianrueil2026.fr)

Total comparateur : 1 327 propositions

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/docs/programmes-candidats-2026.xlsx
+++ b/docs/programmes-candidats-2026.xlsx
@@ -1779,20 +1779,20 @@
       <c r="D29" s="14" t="inlineStr"/>
       <c r="E29" s="17" t="inlineStr">
         <is>
-          <t>https://acteursannecy.fr/</t>
-        </is>
-      </c>
-      <c r="F29" s="21" t="inlineStr">
-        <is>
-          <t>Site identifie</t>
+          <t>https://acteursannecy.fr/programme</t>
+        </is>
+      </c>
+      <c r="F29" s="20" t="inlineStr">
+        <is>
+          <t>Programme complet</t>
         </is>
       </c>
       <c r="G29" s="16" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="H29" s="16" t="inlineStr">
         <is>
-          <t>Non</t>
+          <t>Oui</t>
         </is>
       </c>
     </row>
@@ -1867,20 +1867,20 @@
       <c r="D32" s="14" t="inlineStr"/>
       <c r="E32" s="17" t="inlineStr">
         <is>
-          <t>https://retrouvons-annecy.fr/</t>
-        </is>
-      </c>
-      <c r="F32" s="21" t="inlineStr">
-        <is>
-          <t>Site identifie</t>
+          <t>https://retrouvons-annecy.fr/le-programme/</t>
+        </is>
+      </c>
+      <c r="F32" s="20" t="inlineStr">
+        <is>
+          <t>Programme complet</t>
         </is>
       </c>
       <c r="G32" s="16" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="H32" s="16" t="inlineStr">
         <is>
-          <t>Non</t>
+          <t>Oui</t>
         </is>
       </c>
     </row>
@@ -2159,16 +2159,16 @@
       <c r="D42" s="14" t="inlineStr"/>
       <c r="E42" s="17" t="inlineStr">
         <is>
-          <t>https://www.antonyavenir.fr</t>
-        </is>
-      </c>
-      <c r="F42" s="21" t="inlineStr">
-        <is>
-          <t>Site identifie</t>
+          <t>https://www.antonyavenir.fr/programme</t>
+        </is>
+      </c>
+      <c r="F42" s="15" t="inlineStr">
+        <is>
+          <t>Bien couvert</t>
         </is>
       </c>
       <c r="G42" s="16" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H42" s="16" t="inlineStr">
         <is>
@@ -4467,20 +4467,20 @@
       <c r="D123" s="14" t="inlineStr"/>
       <c r="E123" s="17" t="inlineStr">
         <is>
-          <t>https://brice-bernard.fr/</t>
-        </is>
-      </c>
-      <c r="F123" s="21" t="inlineStr">
-        <is>
-          <t>Site identifie</t>
+          <t>https://brice-bernard.fr/programme.html</t>
+        </is>
+      </c>
+      <c r="F123" s="20" t="inlineStr">
+        <is>
+          <t>Programme complet</t>
         </is>
       </c>
       <c r="G123" s="16" t="n">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="H123" s="16" t="inlineStr">
         <is>
-          <t>Non</t>
+          <t>Oui</t>
         </is>
       </c>
     </row>
@@ -6046,13 +6046,13 @@
           <t>https://www.notreparticestfrejus.fr/</t>
         </is>
       </c>
-      <c r="F178" s="21" t="inlineStr">
-        <is>
-          <t>Site identifie</t>
+      <c r="F178" s="15" t="inlineStr">
+        <is>
+          <t>Bien couvert</t>
         </is>
       </c>
       <c r="G178" s="16" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="H178" s="16" t="inlineStr">
         <is>
@@ -6487,20 +6487,20 @@
       <c r="D193" s="14" t="inlineStr"/>
       <c r="E193" s="17" t="inlineStr">
         <is>
-          <t>https://issyecoloetsocial.fr/</t>
-        </is>
-      </c>
-      <c r="F193" s="21" t="inlineStr">
-        <is>
-          <t>Site identifie</t>
+          <t>https://issyecoloetsocial.fr/notre-programme/</t>
+        </is>
+      </c>
+      <c r="F193" s="20" t="inlineStr">
+        <is>
+          <t>Programme complet</t>
         </is>
       </c>
       <c r="G193" s="16" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="H193" s="16" t="inlineStr">
         <is>
-          <t>Non</t>
+          <t>Oui</t>
         </is>
       </c>
     </row>
@@ -6806,13 +6806,13 @@
           <t>https://josephminniti2026.fr/</t>
         </is>
       </c>
-      <c r="F204" s="21" t="inlineStr">
-        <is>
-          <t>Site identifie</t>
+      <c r="F204" s="15" t="inlineStr">
+        <is>
+          <t>Bien couvert</t>
         </is>
       </c>
       <c r="G204" s="16" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="H204" s="16" t="inlineStr">
         <is>
@@ -6838,13 +6838,13 @@
           <t>https://cheikhmansourmunicipales2026.fr/</t>
         </is>
       </c>
-      <c r="F205" s="21" t="inlineStr">
-        <is>
-          <t>Site identifie</t>
+      <c r="F205" s="15" t="inlineStr">
+        <is>
+          <t>Bien couvert</t>
         </is>
       </c>
       <c r="G205" s="16" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="H205" s="16" t="inlineStr">
         <is>
@@ -13306,13 +13306,13 @@
           <t>https://www.patrickindjianrueil2026.fr/</t>
         </is>
       </c>
-      <c r="F429" s="21" t="inlineStr">
-        <is>
-          <t>Site identifie</t>
+      <c r="F429" s="15" t="inlineStr">
+        <is>
+          <t>Bien couvert</t>
         </is>
       </c>
       <c r="G429" s="16" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="H429" s="16" t="inlineStr">
         <is>
@@ -16439,16 +16439,16 @@
       <c r="D538" s="14" t="inlineStr"/>
       <c r="E538" s="17" t="inlineStr">
         <is>
-          <t>https://pbl2026.fr/</t>
-        </is>
-      </c>
-      <c r="F538" s="21" t="inlineStr">
-        <is>
-          <t>Site identifie</t>
+          <t>https://pbl2026.fr/programme.html</t>
+        </is>
+      </c>
+      <c r="F538" s="15" t="inlineStr">
+        <is>
+          <t>Bien couvert</t>
         </is>
       </c>
       <c r="G538" s="16" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="H538" s="16" t="inlineStr">
         <is>
@@ -16474,13 +16474,13 @@
           <t>https://vitry2026.fr/</t>
         </is>
       </c>
-      <c r="F539" s="21" t="inlineStr">
-        <is>
-          <t>Site identifie</t>
+      <c r="F539" s="15" t="inlineStr">
+        <is>
+          <t>Bien couvert</t>
         </is>
       </c>
       <c r="G539" s="16" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="H539" s="16" t="inlineStr">
         <is>
@@ -16734,13 +16734,13 @@
           <t>https://faridaamrani2026.fr/</t>
         </is>
       </c>
-      <c r="F548" s="21" t="inlineStr">
-        <is>
-          <t>Site identifie</t>
+      <c r="F548" s="15" t="inlineStr">
+        <is>
+          <t>Bien couvert</t>
         </is>
       </c>
       <c r="G548" s="16" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H548" s="16" t="inlineStr">
         <is>
@@ -16947,17 +16947,17 @@
         <v>6</v>
       </c>
       <c r="C6" s="16" t="n">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="D6" s="16" t="n">
         <v>0</v>
       </c>
       <c r="E6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="19" t="inlineStr">
-        <is>
-          <t>En attente</t>
+        <v>2</v>
+      </c>
+      <c r="F6" s="20" t="inlineStr">
+        <is>
+          <t>Programme(s) complet(s)</t>
         </is>
       </c>
     </row>
@@ -16995,7 +16995,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="16" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D8" s="16" t="n">
         <v>0</v>
@@ -17003,9 +17003,9 @@
       <c r="E8" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="F8" s="19" t="inlineStr">
-        <is>
-          <t>En attente</t>
+      <c r="F8" s="18" t="inlineStr">
+        <is>
+          <t>Partiellement couvert</t>
         </is>
       </c>
     </row>
@@ -17403,17 +17403,17 @@
         <v>7</v>
       </c>
       <c r="C25" s="16" t="n">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="D25" s="16" t="n">
         <v>0</v>
       </c>
       <c r="E25" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="F25" s="19" t="inlineStr">
-        <is>
-          <t>En attente</t>
+        <v>1</v>
+      </c>
+      <c r="F25" s="20" t="inlineStr">
+        <is>
+          <t>Programme(s) complet(s)</t>
         </is>
       </c>
     </row>
@@ -17715,7 +17715,7 @@
         <v>6</v>
       </c>
       <c r="C38" s="16" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="D38" s="16" t="n">
         <v>0</v>
@@ -17723,9 +17723,9 @@
       <c r="E38" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="F38" s="19" t="inlineStr">
-        <is>
-          <t>En attente</t>
+      <c r="F38" s="18" t="inlineStr">
+        <is>
+          <t>Partiellement couvert</t>
         </is>
       </c>
     </row>
@@ -17763,17 +17763,17 @@
         <v>3</v>
       </c>
       <c r="C40" s="16" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="D40" s="16" t="n">
         <v>0</v>
       </c>
       <c r="E40" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="F40" s="19" t="inlineStr">
-        <is>
-          <t>En attente</t>
+        <v>1</v>
+      </c>
+      <c r="F40" s="20" t="inlineStr">
+        <is>
+          <t>Programme(s) complet(s)</t>
         </is>
       </c>
     </row>
@@ -17835,7 +17835,7 @@
         <v>5</v>
       </c>
       <c r="C43" s="16" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="D43" s="16" t="n">
         <v>0</v>
@@ -17843,9 +17843,9 @@
       <c r="E43" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="F43" s="19" t="inlineStr">
-        <is>
-          <t>En attente</t>
+      <c r="F43" s="15" t="inlineStr">
+        <is>
+          <t>Bien couvert</t>
         </is>
       </c>
     </row>
@@ -18771,7 +18771,7 @@
         <v>2</v>
       </c>
       <c r="C82" s="16" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D82" s="16" t="n">
         <v>0</v>
@@ -18779,9 +18779,9 @@
       <c r="E82" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="F82" s="19" t="inlineStr">
-        <is>
-          <t>En attente</t>
+      <c r="F82" s="18" t="inlineStr">
+        <is>
+          <t>Partiellement couvert</t>
         </is>
       </c>
     </row>
@@ -19227,7 +19227,7 @@
         <v>3</v>
       </c>
       <c r="C101" s="16" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="D101" s="16" t="n">
         <v>0</v>
@@ -19235,9 +19235,9 @@
       <c r="E101" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="F101" s="19" t="inlineStr">
-        <is>
-          <t>En attente</t>
+      <c r="F101" s="15" t="inlineStr">
+        <is>
+          <t>Bien couvert</t>
         </is>
       </c>
     </row>
@@ -19299,7 +19299,7 @@
         <v>3</v>
       </c>
       <c r="C104" s="16" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D104" s="16" t="n">
         <v>0</v>
@@ -19307,9 +19307,9 @@
       <c r="E104" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="F104" s="19" t="inlineStr">
-        <is>
-          <t>En attente</t>
+      <c r="F104" s="18" t="inlineStr">
+        <is>
+          <t>Partiellement couvert</t>
         </is>
       </c>
     </row>

</xml_diff>